<commit_message>
Update to downloadable table
</commit_message>
<xml_diff>
--- a/output/Serengeti_Rabies_Incidence.xlsx
+++ b/output/Serengeti_Rabies_Incidence.xlsx
@@ -21,8 +21,7 @@
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>This data is from the XXX. Please cite (YYY) if used.
-                  For more information, please contact: ZZZ</t>
+    <t>This data is from the XXX. Please cite (YYY) if used. For more information, please contact Katie Hampson (Katie.Hampson@glasgow.ac.uk)</t>
   </si>
   <si>
     <t>Year</t>
@@ -161,7 +160,7 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <sz val="14.0"/>
+      <sz val="12.0"/>
       <color rgb="000000"/>
       <b val="true"/>
     </font>
@@ -432,12 +431,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="14.0" customWidth="true"/>
-    <col min="2" max="2" width="14.0" customWidth="true"/>
-    <col min="3" max="3" width="14.0" customWidth="true"/>
-    <col min="4" max="4" width="14.0" customWidth="true"/>
-    <col min="5" max="5" width="14.0" customWidth="true"/>
-    <col min="6" max="6" width="14.0" customWidth="true"/>
+    <col min="1" max="1" width="20.0" customWidth="true"/>
+    <col min="2" max="2" width="20.0" customWidth="true"/>
+    <col min="3" max="3" width="20.0" customWidth="true"/>
+    <col min="4" max="4" width="20.0" customWidth="true"/>
+    <col min="5" max="5" width="20.0" customWidth="true"/>
+    <col min="6" max="6" width="20.0" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -749,7 +748,7 @@
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="B3:G7"/>
+    <mergeCell ref="B3:E7"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -763,14 +762,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="14.0" customWidth="true"/>
-    <col min="2" max="2" width="14.0" customWidth="true"/>
-    <col min="3" max="3" width="14.0" customWidth="true"/>
-    <col min="4" max="4" width="14.0" customWidth="true"/>
-    <col min="5" max="5" width="14.0" customWidth="true"/>
-    <col min="6" max="6" width="14.0" customWidth="true"/>
-    <col min="7" max="7" width="14.0" customWidth="true"/>
-    <col min="8" max="8" width="14.0" customWidth="true"/>
+    <col min="1" max="1" width="20.0" customWidth="true"/>
+    <col min="2" max="2" width="20.0" customWidth="true"/>
+    <col min="3" max="3" width="20.0" customWidth="true"/>
+    <col min="4" max="4" width="20.0" customWidth="true"/>
+    <col min="5" max="5" width="20.0" customWidth="true"/>
+    <col min="6" max="6" width="20.0" customWidth="true"/>
+    <col min="7" max="7" width="20.0" customWidth="true"/>
+    <col min="8" max="8" width="20.0" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>